<commit_message>
game data tool fix
</commit_message>
<xml_diff>
--- a/GameDataConfigTool/excels/AccountTest.xlsx
+++ b/GameDataConfigTool/excels/AccountTest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\UnityProjects\SynthMind\GameDataConfigTool\excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\SynthMind\GameDataConfigTool\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1ABEF0-0FF6-422C-8183-40BB0435DE97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1351A86E-3BCE-4001-97E4-77E9EB3AD2FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14880" yWindow="7500" windowWidth="17130" windowHeight="10680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3195" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>id|int</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>YKH</t>
+  </si>
+  <si>
+    <t>isAI|bool</t>
   </si>
 </sst>
 </file>
@@ -392,24 +395,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -417,61 +421,67 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
       <c r="D2" t="s">
         <v>11</v>
       </c>
       <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" t="s">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
         <v>8</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{B22AEC7F-0E85-433E-9A25-D7832D11FD53}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{B22AEC7F-0E85-433E-9A25-D7832D11FD53}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>